<commit_message>
Padel: new for loops
</commit_message>
<xml_diff>
--- a/Bocetos.xlsx
+++ b/Bocetos.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Documentos\Programas\eclipse\reservasDeportivas\DeportiveApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D5E20B-8FBC-4028-BCDE-41108708BFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBF341B-CE14-47AE-A571-309ED2E37581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2088" yWindow="3648" windowWidth="17280" windowHeight="8964" xr2:uid="{A76B02FD-D3D2-4A8F-BE6D-2C8775B3965A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A76B02FD-D3D2-4A8F-BE6D-2C8775B3965A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>INTERFACES</t>
   </si>
@@ -105,14 +105,64 @@
   </si>
   <si>
     <t>Hora para hacer dxt máx</t>
+  </si>
+  <si>
+    <t>Usuarios</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Empleo</t>
+  </si>
+  <si>
+    <t>Acrónimo (PK)</t>
+  </si>
+  <si>
+    <t>Apellido_1</t>
+  </si>
+  <si>
+    <t>Apellido_2</t>
+  </si>
+  <si>
+    <t>Deportes</t>
+  </si>
+  <si>
+    <t>id_Deporte (PK)</t>
+  </si>
+  <si>
+    <t>Nombre_deporte</t>
+  </si>
+  <si>
+    <t>Acrónimo (FK)</t>
+  </si>
+  <si>
+    <t>Id_Deporte (FK)</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Hora</t>
+  </si>
+  <si>
+    <t>Reservas (N:M)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -140,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -149,6 +199,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -465,13 +518,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D76B8CF-B8E8-4616-9A38-54560FF28E41}">
-  <dimension ref="B1:L16"/>
+  <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
@@ -682,7 +740,9 @@
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -693,9 +753,15 @@
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="B16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -703,10 +769,54 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>